<commit_message>
Implementando as funções add, remove e busca
</commit_message>
<xml_diff>
--- a/Clientes.xlsx
+++ b/Clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lipi-\OneDrive\Documentos\GitHub\DP--CC4651--Empresa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="11_AD4D361C20488DEA4E38A0B1BC5E7FAC5ADEDD9D" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5708BA5A-654E-4D34-8C2A-A6DC441E49C0}"/>
+  <xr:revisionPtr revIDLastSave="253" documentId="11_AD4D361C20488DEA4E38A0B1BC5E7FAC5ADEDD9D" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E93B4144-3247-4167-BDAD-FD2FCF88F82A}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="74">
   <si>
     <t>Nome</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>Endereco</t>
+  </si>
+  <si>
+    <t>Codigo</t>
   </si>
 </sst>
 </file>
@@ -333,7 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -352,6 +355,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -635,15 +641,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
@@ -652,532 +656,601 @@
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>18</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>666</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>120</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>666</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>115</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>666</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>18</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>356</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="3">
         <v>21</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>420</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>20</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>891</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>20</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>21</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <v>21</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>657</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="3">
         <v>18</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="3">
+      <c r="D11" s="3">
         <v>18</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>55</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="3">
+      <c r="D12" s="3">
         <v>18</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>120</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="3">
+      <c r="D13" s="3">
         <v>18</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>200</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="3">
         <v>18</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>55</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="3">
         <v>18</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <v>222</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="3">
+      <c r="D16" s="3">
         <v>850</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="3">
+      <c r="D17" s="3">
         <v>23</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="3">
+      <c r="G17" s="3">
         <v>100</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="3">
+      <c r="D18" s="3">
         <v>21</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="3">
+      <c r="G18" s="3">
         <v>52</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="3">
+      <c r="D19" s="3">
         <v>21</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="3">
+      <c r="G19" s="3">
         <v>63</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="H19" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="3">
+      <c r="D20" s="3">
         <v>21</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="3">
+      <c r="G20" s="3">
         <v>150</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="H20" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="3">
+      <c r="D21" s="3">
         <v>21</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="3">
+      <c r="G21" s="3">
         <v>215</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="H21" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="3">
+      <c r="D22" s="3">
         <v>21</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="3">
+      <c r="G22" s="3">
         <v>212</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="H22" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="3">
+      <c r="D23" s="3">
         <v>21</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="3">
+      <c r="G23" s="3">
         <v>415</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="H23" s="6" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>